<commit_message>
Atualiza conforme deliberação 17 e 18
</commit_message>
<xml_diff>
--- a/upload/projetos_acordo_judicial_reparacao_vale.xlsx
+++ b/upload/projetos_acordo_judicial_reparacao_vale.xlsx
@@ -1,9 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27230"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27718"/>
   <workbookPr hidePivotFieldList="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F1DB50D-1627-4396-AF5D-1DC9D5ABA7E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD53CBF0-9A17-4DAF-89F6-9783E39AF004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="10320" windowHeight="7560" tabRatio="867" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -14,10 +19,12 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">projetos!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">projetos!$A$1:$H$61</definedName>
     <definedName name="check">#REF!</definedName>
-    <definedName name="deliberacao12">projetos!$G$2:$H$61</definedName>
+    <definedName name="deli">projetos!#REF!</definedName>
+    <definedName name="deliberacao12">projetos!#REF!</definedName>
     <definedName name="projetos">'[1]Tabela 1 - Projetos com valor'!$C$4:$D$64</definedName>
+    <definedName name="SITE">projetos!$B$2:$D$61</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -204,9 +211,6 @@
     <t>Conclusão de obra e Equipagem de Hospitais Regionais</t>
   </si>
   <si>
-    <t>Estudo de viabilidade técnica e financeira e modelo de gestão da reestruturação da Fundação Ezequiel Dias – Funed</t>
-  </si>
-  <si>
     <t>Elaboração de instrumentos de gestão para desenvolvimento de mineração sustentável e competitiva - Avaliação Ambiental Estratégica</t>
   </si>
   <si>
@@ -222,9 +226,6 @@
     <t>Implantação de Fábrica de Software para construção de sistema de governança ambiental</t>
   </si>
   <si>
-    <t>Estruturação, reforma e ampliação da Fundação Ezequiel Dias – Funed</t>
-  </si>
-  <si>
     <t>Plano de Desenvolvimento da Cadeia Agropecuária</t>
   </si>
   <si>
@@ -253,6 +254,12 @@
   </si>
   <si>
     <t>I.3</t>
+  </si>
+  <si>
+    <t>Construção e manutenção de um Novo Complexo de Saúde e operação de serviços não assistenciais/laboratoriais</t>
+  </si>
+  <si>
+    <t>Melhoria da infraestrutura dos municípios – Adequação de serviços de transporte fluvial em Morada Nova de Minas</t>
   </si>
 </sst>
 </file>
@@ -299,15 +306,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -323,7 +327,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -624,28 +628,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E63"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="62.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="45" style="4" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="4" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="4"/>
-    <col min="8" max="8" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="9.140625" style="4"/>
-    <col min="12" max="12" width="9.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="14.28515625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="62.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="45" style="3" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" style="6" customWidth="1"/>
+    <col min="5" max="7" width="9.140625" style="3"/>
+    <col min="8" max="8" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -655,12 +655,12 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A2" s="5">
+    <row r="2" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A2" s="4">
         <v>9288130</v>
       </c>
       <c r="B2" t="s">
@@ -669,13 +669,12 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>1195796000</v>
       </c>
-      <c r="E2" s="9"/>
-    </row>
-    <row r="3" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A3" s="5">
+    </row>
+    <row r="3" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A3" s="4">
         <v>9288130</v>
       </c>
       <c r="B3" t="s">
@@ -684,13 +683,12 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>450000000</v>
       </c>
-      <c r="E3" s="9"/>
-    </row>
-    <row r="4" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A4" s="5">
+    </row>
+    <row r="4" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A4" s="4">
         <v>9288132</v>
       </c>
       <c r="B4" t="s">
@@ -699,13 +697,12 @@
       <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>270000000</v>
       </c>
-      <c r="E4" s="9"/>
-    </row>
-    <row r="5" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A5" s="5">
+    </row>
+    <row r="5" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A5" s="4">
         <v>9288133</v>
       </c>
       <c r="B5" t="s">
@@ -714,13 +711,12 @@
       <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>776000000</v>
       </c>
-      <c r="E5" s="9"/>
-    </row>
-    <row r="6" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A6" s="5">
+    </row>
+    <row r="6" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A6" s="4">
         <v>9288134</v>
       </c>
       <c r="B6" t="s">
@@ -729,13 +725,12 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>118860000</v>
       </c>
-      <c r="E6" s="9"/>
-    </row>
-    <row r="7" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="5">
+    </row>
+    <row r="7" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A7" s="4">
         <v>9288135</v>
       </c>
       <c r="B7" t="s">
@@ -744,13 +739,12 @@
       <c r="C7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>1345000</v>
       </c>
-      <c r="E7" s="9"/>
-    </row>
-    <row r="8" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A8" s="5">
+    </row>
+    <row r="8" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A8" s="4">
         <v>9288136</v>
       </c>
       <c r="B8" t="s">
@@ -759,13 +753,12 @@
       <c r="C8" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>111480000</v>
       </c>
-      <c r="E8" s="9"/>
-    </row>
-    <row r="9" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A9" s="5">
+    </row>
+    <row r="9" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A9" s="4">
         <v>9288137</v>
       </c>
       <c r="B9" t="s">
@@ -774,13 +767,12 @@
       <c r="C9" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>98100000</v>
       </c>
-      <c r="E9" s="9"/>
-    </row>
-    <row r="10" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A10" s="5">
+    </row>
+    <row r="10" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A10" s="4">
         <v>9288138</v>
       </c>
       <c r="B10" t="s">
@@ -789,13 +781,12 @@
       <c r="C10" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>38614000</v>
       </c>
-      <c r="E10" s="9"/>
-    </row>
-    <row r="11" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A11" s="5">
+    </row>
+    <row r="11" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A11" s="4">
         <v>9288139</v>
       </c>
       <c r="B11" t="s">
@@ -804,13 +795,12 @@
       <c r="C11" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>3200000</v>
       </c>
-      <c r="E11" s="9"/>
-    </row>
-    <row r="12" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A12" s="5">
+    </row>
+    <row r="12" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A12" s="4">
         <v>9288141</v>
       </c>
       <c r="B12" t="s">
@@ -819,13 +809,12 @@
       <c r="C12" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>500000</v>
       </c>
-      <c r="E12" s="9"/>
-    </row>
-    <row r="13" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A13" s="5">
+    </row>
+    <row r="13" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A13" s="4">
         <v>9288142</v>
       </c>
       <c r="B13" t="s">
@@ -834,13 +823,12 @@
       <c r="C13" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <v>29712000</v>
       </c>
-      <c r="E13" s="9"/>
-    </row>
-    <row r="14" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A14" s="5">
+    </row>
+    <row r="14" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A14" s="4">
         <v>9288143</v>
       </c>
       <c r="B14" t="s">
@@ -849,13 +837,12 @@
       <c r="C14" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <v>728000</v>
       </c>
-      <c r="E14" s="9"/>
-    </row>
-    <row r="15" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A15" s="5">
+    </row>
+    <row r="15" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A15" s="4">
         <v>9288144</v>
       </c>
       <c r="B15" t="s">
@@ -864,13 +851,12 @@
       <c r="C15" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="5">
         <v>49000000</v>
       </c>
-      <c r="E15" s="9"/>
-    </row>
-    <row r="16" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A16" s="5">
+    </row>
+    <row r="16" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A16" s="4">
         <v>9288145</v>
       </c>
       <c r="B16" t="s">
@@ -879,13 +865,12 @@
       <c r="C16" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="5">
         <v>45345000</v>
       </c>
-      <c r="E16" s="9"/>
-    </row>
-    <row r="17" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A17" s="5">
+    </row>
+    <row r="17" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A17" s="4">
         <v>9288147</v>
       </c>
       <c r="B17" t="s">
@@ -894,13 +879,12 @@
       <c r="C17" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="5">
         <v>14817323</v>
       </c>
-      <c r="E17" s="9"/>
-    </row>
-    <row r="18" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A18" s="5">
+    </row>
+    <row r="18" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A18" s="4">
         <v>9288148</v>
       </c>
       <c r="B18" t="s">
@@ -909,13 +893,12 @@
       <c r="C18" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="6">
+      <c r="D18" s="5">
         <v>4000000</v>
       </c>
-      <c r="E18" s="9"/>
-    </row>
-    <row r="19" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A19" s="5">
+    </row>
+    <row r="19" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A19" s="4">
         <v>9288149</v>
       </c>
       <c r="B19" t="s">
@@ -924,13 +907,12 @@
       <c r="C19" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="5">
         <v>5000000</v>
       </c>
-      <c r="E19" s="9"/>
-    </row>
-    <row r="20" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A20" s="5">
+    </row>
+    <row r="20" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A20" s="4">
         <v>9288150</v>
       </c>
       <c r="B20" t="s">
@@ -939,13 +921,12 @@
       <c r="C20" t="s">
         <v>5</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="5">
         <v>10671300</v>
       </c>
-      <c r="E20" s="9"/>
-    </row>
-    <row r="21" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A21" s="5">
+    </row>
+    <row r="21" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A21" s="4">
         <v>9288152</v>
       </c>
       <c r="B21" t="s">
@@ -954,13 +935,12 @@
       <c r="C21" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="5">
         <v>15130000</v>
       </c>
-      <c r="E21" s="9"/>
-    </row>
-    <row r="22" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A22" s="5">
+    </row>
+    <row r="22" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A22" s="4">
         <v>9288153</v>
       </c>
       <c r="B22" t="s">
@@ -969,13 +949,12 @@
       <c r="C22" t="s">
         <v>5</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="5">
         <v>3000000</v>
       </c>
-      <c r="E22" s="9"/>
-    </row>
-    <row r="23" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A23" s="5">
+    </row>
+    <row r="23" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A23" s="4">
         <v>9288154</v>
       </c>
       <c r="B23" t="s">
@@ -984,13 +963,12 @@
       <c r="C23" t="s">
         <v>5</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="5">
         <v>650000</v>
       </c>
-      <c r="E23" s="9"/>
-    </row>
-    <row r="24" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A24" s="5">
+    </row>
+    <row r="24" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A24" s="4">
         <v>9288155</v>
       </c>
       <c r="B24" t="s">
@@ -999,13 +977,12 @@
       <c r="C24" t="s">
         <v>5</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="5">
         <v>5550438.4000000004</v>
       </c>
-      <c r="E24" s="9"/>
-    </row>
-    <row r="25" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A25" s="5">
+    </row>
+    <row r="25" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A25" s="4">
         <v>9288167</v>
       </c>
       <c r="B25" t="s">
@@ -1014,13 +991,12 @@
       <c r="C25" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="5">
         <v>3773400</v>
       </c>
-      <c r="E25" s="9"/>
-    </row>
-    <row r="26" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A26" s="5">
+    </row>
+    <row r="26" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A26" s="4">
         <v>9288168</v>
       </c>
       <c r="B26" t="s">
@@ -1029,13 +1005,12 @@
       <c r="C26" t="s">
         <v>5</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="5">
         <v>130000000</v>
       </c>
-      <c r="E26" s="9"/>
-    </row>
-    <row r="27" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A27" s="5">
+    </row>
+    <row r="27" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A27" s="4">
         <v>9288169</v>
       </c>
       <c r="B27" t="s">
@@ -1044,13 +1019,12 @@
       <c r="C27" t="s">
         <v>5</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="5">
         <v>16112602.23</v>
       </c>
-      <c r="E27" s="9"/>
-    </row>
-    <row r="28" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A28" s="5">
+    </row>
+    <row r="28" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A28" s="4">
         <v>9288176</v>
       </c>
       <c r="B28" t="s">
@@ -1059,13 +1033,12 @@
       <c r="C28" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="5">
         <v>31729352.109999999</v>
       </c>
-      <c r="E28" s="9"/>
-    </row>
-    <row r="29" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A29" s="5">
+    </row>
+    <row r="29" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A29" s="4">
         <v>9288177</v>
       </c>
       <c r="B29" t="s">
@@ -1074,13 +1047,12 @@
       <c r="C29" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="5">
         <v>0</v>
       </c>
-      <c r="E29" s="9"/>
-    </row>
-    <row r="30" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A30" s="5">
+    </row>
+    <row r="30" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A30" s="4">
         <v>9288178</v>
       </c>
       <c r="B30" t="s">
@@ -1089,13 +1061,12 @@
       <c r="C30" t="s">
         <v>5</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D30" s="5">
         <v>253000000</v>
       </c>
-      <c r="E30" s="9"/>
-    </row>
-    <row r="31" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A31" s="5">
+    </row>
+    <row r="31" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A31" s="4">
         <v>9288179</v>
       </c>
       <c r="B31" t="s">
@@ -1104,13 +1075,12 @@
       <c r="C31" t="s">
         <v>5</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="5">
         <v>45000000</v>
       </c>
-      <c r="E31" s="9"/>
-    </row>
-    <row r="32" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A32" s="5">
+    </row>
+    <row r="32" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A32" s="4">
         <v>9288180</v>
       </c>
       <c r="B32" t="s">
@@ -1119,13 +1089,12 @@
       <c r="C32" t="s">
         <v>7</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32" s="5">
         <v>3072030000</v>
       </c>
-      <c r="E32" s="9"/>
-    </row>
-    <row r="33" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A33" s="5">
+    </row>
+    <row r="33" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A33" s="4">
         <v>9288181</v>
       </c>
       <c r="B33" t="s">
@@ -1134,13 +1103,12 @@
       <c r="C33" t="s">
         <v>5</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33" s="5">
         <v>75352000</v>
       </c>
-      <c r="E33" s="9"/>
-    </row>
-    <row r="34" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A34" s="5">
+    </row>
+    <row r="34" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A34" s="4">
         <v>9288182</v>
       </c>
       <c r="B34" t="s">
@@ -1149,13 +1117,12 @@
       <c r="C34" t="s">
         <v>5</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34" s="5">
         <v>7000000</v>
       </c>
-      <c r="E34" s="9"/>
-    </row>
-    <row r="35" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A35" s="5">
+    </row>
+    <row r="35" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A35" s="4">
         <v>9288183</v>
       </c>
       <c r="B35" t="s">
@@ -1164,13 +1131,12 @@
       <c r="C35" t="s">
         <v>5</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35" s="5">
         <v>9302249.2699999996</v>
       </c>
-      <c r="E35" s="9"/>
-    </row>
-    <row r="36" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A36" s="5">
+    </row>
+    <row r="36" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A36" s="4">
         <v>9288185</v>
       </c>
       <c r="B36" t="s">
@@ -1179,13 +1145,12 @@
       <c r="C36" t="s">
         <v>5</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D36" s="5">
         <v>2000000</v>
       </c>
-      <c r="E36" s="9"/>
-    </row>
-    <row r="37" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A37" s="5">
+    </row>
+    <row r="37" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A37" s="4">
         <v>9288186</v>
       </c>
       <c r="B37" t="s">
@@ -1194,13 +1159,12 @@
       <c r="C37" t="s">
         <v>5</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D37" s="5">
         <v>3000000</v>
       </c>
-      <c r="E37" s="9"/>
-    </row>
-    <row r="38" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A38" s="5">
+    </row>
+    <row r="38" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A38" s="4">
         <v>9288187</v>
       </c>
       <c r="B38" t="s">
@@ -1209,13 +1173,12 @@
       <c r="C38" t="s">
         <v>5</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D38" s="5">
         <v>36000000</v>
       </c>
-      <c r="E38" s="9"/>
-    </row>
-    <row r="39" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A39" s="5">
+    </row>
+    <row r="39" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A39" s="4">
         <v>9288188</v>
       </c>
       <c r="B39" t="s">
@@ -1224,13 +1187,12 @@
       <c r="C39" t="s">
         <v>5</v>
       </c>
-      <c r="D39" s="6">
+      <c r="D39" s="5">
         <v>8647600</v>
       </c>
-      <c r="E39" s="9"/>
-    </row>
-    <row r="40" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A40" s="5">
+    </row>
+    <row r="40" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A40" s="4">
         <v>9288189</v>
       </c>
       <c r="B40" t="s">
@@ -1239,13 +1201,12 @@
       <c r="C40" t="s">
         <v>5</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D40" s="5">
         <v>300000</v>
       </c>
-      <c r="E40" s="9"/>
-    </row>
-    <row r="41" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A41" s="5">
+    </row>
+    <row r="41" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A41" s="4">
         <v>9288190</v>
       </c>
       <c r="B41" t="s">
@@ -1254,13 +1215,12 @@
       <c r="C41" t="s">
         <v>45</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D41" s="5">
         <v>100000000</v>
       </c>
-      <c r="E41" s="9"/>
-    </row>
-    <row r="42" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A42" s="5">
+    </row>
+    <row r="42" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A42" s="4">
         <v>9288191</v>
       </c>
       <c r="B42" t="s">
@@ -1269,13 +1229,12 @@
       <c r="C42" t="s">
         <v>47</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D42" s="5">
         <v>210000000</v>
       </c>
-      <c r="E42" s="9"/>
-    </row>
-    <row r="43" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A43" s="5">
+    </row>
+    <row r="43" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A43" s="4">
         <v>9288192</v>
       </c>
       <c r="B43" t="s">
@@ -1284,13 +1243,12 @@
       <c r="C43" t="s">
         <v>47</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D43" s="5">
         <v>100000000</v>
       </c>
-      <c r="E43" s="9"/>
-    </row>
-    <row r="44" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A44" s="5">
+    </row>
+    <row r="44" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A44" s="4">
         <v>9288193</v>
       </c>
       <c r="B44" t="s">
@@ -1299,13 +1257,12 @@
       <c r="C44" t="s">
         <v>5</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D44" s="5">
         <v>3900000</v>
       </c>
-      <c r="E44" s="9"/>
-    </row>
-    <row r="45" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A45" s="5">
+    </row>
+    <row r="45" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A45" s="4">
         <v>9288194</v>
       </c>
       <c r="B45" t="s">
@@ -1314,13 +1271,12 @@
       <c r="C45" t="s">
         <v>5</v>
       </c>
-      <c r="D45" s="6">
+      <c r="D45" s="5">
         <v>3600000</v>
       </c>
-      <c r="E45" s="9"/>
-    </row>
-    <row r="46" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A46" s="5">
+    </row>
+    <row r="46" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A46" s="4">
         <v>9288195</v>
       </c>
       <c r="B46" t="s">
@@ -1329,13 +1285,12 @@
       <c r="C46" t="s">
         <v>5</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D46" s="5">
         <v>749679</v>
       </c>
-      <c r="E46" s="9"/>
-    </row>
-    <row r="47" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A47" s="5">
+    </row>
+    <row r="47" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A47" s="4">
         <v>9288196</v>
       </c>
       <c r="B47" t="s">
@@ -1344,13 +1299,12 @@
       <c r="C47" t="s">
         <v>5</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D47" s="5">
         <v>42412000</v>
       </c>
-      <c r="E47" s="9"/>
-    </row>
-    <row r="48" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A48" s="5">
+    </row>
+    <row r="48" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A48" s="4">
         <v>9288198</v>
       </c>
       <c r="B48" t="s">
@@ -1359,14 +1313,13 @@
       <c r="C48" t="s">
         <v>5</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D48" s="5">
         <v>986059044</v>
       </c>
-      <c r="E48" s="9"/>
-    </row>
-    <row r="49" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A49" s="5">
-        <v>9288209</v>
+    </row>
+    <row r="49" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A49" s="4">
+        <v>9288210</v>
       </c>
       <c r="B49" t="s">
         <v>54</v>
@@ -1374,14 +1327,13 @@
       <c r="C49" t="s">
         <v>5</v>
       </c>
-      <c r="D49" s="6">
-        <v>1200000</v>
-      </c>
-      <c r="E49" s="9"/>
-    </row>
-    <row r="50" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A50" s="5">
-        <v>9288210</v>
+      <c r="D49" s="5">
+        <v>2500000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A50" s="4">
+        <v>9288211</v>
       </c>
       <c r="B50" t="s">
         <v>55</v>
@@ -1389,44 +1341,41 @@
       <c r="C50" t="s">
         <v>5</v>
       </c>
-      <c r="D50" s="6">
-        <v>2500000</v>
-      </c>
-      <c r="E50" s="9"/>
-    </row>
-    <row r="51" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A51" s="5">
-        <v>9288211</v>
+      <c r="D50" s="5">
+        <v>3200000</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A51" s="4">
+        <v>9288212</v>
       </c>
       <c r="B51" t="s">
         <v>56</v>
       </c>
       <c r="C51" t="s">
-        <v>5</v>
-      </c>
-      <c r="D51" s="6">
-        <v>3200000</v>
-      </c>
-      <c r="E51" s="9"/>
-    </row>
-    <row r="52" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A52" s="5">
-        <v>9288212</v>
+        <v>57</v>
+      </c>
+      <c r="D51" s="5">
+        <v>2427295557.8899999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A52" s="4">
+        <v>9288213</v>
       </c>
       <c r="B52" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C52" t="s">
-        <v>58</v>
-      </c>
-      <c r="D52" s="6">
-        <v>2427295557.8899999</v>
-      </c>
-      <c r="E52" s="9"/>
-    </row>
-    <row r="53" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A53" s="5">
-        <v>9288213</v>
+        <v>5</v>
+      </c>
+      <c r="D52" s="5">
+        <v>23000005</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A53" s="4">
+        <v>9321270</v>
       </c>
       <c r="B53" t="s">
         <v>59</v>
@@ -1434,163 +1383,154 @@
       <c r="C53" t="s">
         <v>5</v>
       </c>
-      <c r="D53" s="6">
-        <v>23000005</v>
-      </c>
-      <c r="E53" s="9"/>
-    </row>
-    <row r="54" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A54" s="5">
-        <v>9288214</v>
+      <c r="D53" s="5">
+        <v>842212.06</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A54">
+        <v>9334530</v>
       </c>
       <c r="B54" t="s">
         <v>60</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D54" s="6">
-        <v>199489167.000002</v>
-      </c>
-      <c r="E54" s="9"/>
-    </row>
-    <row r="55" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A55" s="5">
-        <v>9321270</v>
+        <v>14000000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A55">
+        <v>9337957</v>
       </c>
       <c r="B55" t="s">
         <v>61</v>
       </c>
       <c r="C55" t="s">
-        <v>5</v>
-      </c>
-      <c r="D55" s="6">
-        <v>842212.06</v>
-      </c>
-      <c r="E55" s="9"/>
-    </row>
-    <row r="56" spans="1:5" ht="20.100000000000001" customHeight="1">
+        <v>7</v>
+      </c>
+      <c r="D55" s="5">
+        <v>470156273.05000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A56">
-        <v>9334530</v>
+        <v>9341846</v>
       </c>
       <c r="B56" t="s">
         <v>62</v>
       </c>
-      <c r="C56" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D56" s="7">
-        <v>14000000</v>
-      </c>
-      <c r="E56" s="9"/>
-    </row>
-    <row r="57" spans="1:5" ht="20.100000000000001" customHeight="1">
+      <c r="C56" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" s="5">
+        <v>13900000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="20.100000000000001" customHeight="1">
       <c r="A57">
-        <v>9337957</v>
+        <v>9342884</v>
       </c>
       <c r="B57" t="s">
         <v>63</v>
       </c>
       <c r="C57" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" s="5">
+        <v>68000000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A58" s="7">
+        <v>9361779</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C58" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D57" s="6">
-        <v>470156273.05000001</v>
-      </c>
-      <c r="E57" s="9"/>
-    </row>
-    <row r="58" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A58">
-        <v>9341846</v>
-      </c>
-      <c r="B58" t="s">
-        <v>64</v>
-      </c>
-      <c r="C58" t="s">
-        <v>5</v>
-      </c>
       <c r="D58" s="6">
-        <v>13900000</v>
-      </c>
-      <c r="E58" s="9"/>
-    </row>
-    <row r="59" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A59">
-        <v>9342884</v>
-      </c>
-      <c r="B59" t="s">
+        <v>164460000</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="A59" s="7">
+        <v>9345390</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D59" s="6">
-        <v>68000000</v>
-      </c>
-      <c r="E59" s="9"/>
-    </row>
-    <row r="60" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A60" s="8">
-        <v>9361779</v>
-      </c>
-      <c r="B60" s="4" t="s">
+        <v>24164127.77</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="30">
+      <c r="A60" s="7">
+        <v>9345097</v>
+      </c>
+      <c r="B60" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C60" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D60" s="7">
-        <v>164460000</v>
-      </c>
-      <c r="E60" s="9"/>
-    </row>
-    <row r="61" spans="1:5" ht="20.100000000000001" customHeight="1">
-      <c r="A61" s="8">
-        <v>9345390</v>
-      </c>
-      <c r="B61" s="4" t="s">
+      <c r="C60" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" s="6">
+        <v>3091752</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="30">
+      <c r="A61" s="7">
+        <v>9395028</v>
+      </c>
+      <c r="B61" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C61" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D61" s="7">
-        <v>24164127.77</v>
-      </c>
-      <c r="E61" s="9"/>
-    </row>
-    <row r="62" spans="1:5" ht="30.75">
-      <c r="A62" s="8">
-        <v>9345097</v>
-      </c>
-      <c r="B62" s="4" t="s">
+      <c r="C61" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C62" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D62" s="7">
-        <v>3091752</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="30.75">
-      <c r="A63" s="8">
-        <v>9395028</v>
-      </c>
-      <c r="B63" s="4" t="s">
+      <c r="D61" s="6">
+        <v>262717753.97999999</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="30.75">
+      <c r="A62" s="7">
+        <v>9428110</v>
+      </c>
+      <c r="B62" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C63" s="4" t="s">
+      <c r="C62" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62" s="8">
+        <v>200689167</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="30.75">
+      <c r="A63" s="7">
+        <v>9428104</v>
+      </c>
+      <c r="B63" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D63" s="7">
-        <v>262717753.97999999</v>
+      <c r="C63" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" s="6">
+        <v>6000000</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L62" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D60">
-    <sortCondition ref="A1:A60"/>
+  <autoFilter ref="A1:H63" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D58">
+    <sortCondition ref="A1:A58"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Atualiza conforme deliberação 19
</commit_message>
<xml_diff>
--- a/upload/projetos_acordo_judicial_reparacao_vale.xlsx
+++ b/upload/projetos_acordo_judicial_reparacao_vale.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27718"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27804"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD53CBF0-9A17-4DAF-89F6-9783E39AF004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FDE99D85-FE68-4207-BD74-C86C09F0F68F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="10320" windowHeight="7560" tabRatio="867" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,9 +20,6 @@
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">projetos!$A$1:$H$61</definedName>
-    <definedName name="check">#REF!</definedName>
-    <definedName name="deli">projetos!#REF!</definedName>
-    <definedName name="deliberacao12">projetos!#REF!</definedName>
     <definedName name="projetos">'[1]Tabela 1 - Projetos com valor'!$C$4:$D$64</definedName>
     <definedName name="SITE">projetos!$B$2:$D$61</definedName>
   </definedNames>
@@ -94,7 +91,7 @@
     <t>Proteção policial individual e do cidadão mineiro</t>
   </si>
   <si>
-    <t>Atualização do Plano Diretor de Desenvolvimento Integrado da Região Metropolitana de Belo Horizonte - PDDI-RMBH</t>
+    <t>Atualização do Plano de Desenvolvimento Urbano Integrado da Região Metropolitana de Belo Horizonte – PDUI-RMBH</t>
   </si>
   <si>
     <t>Georreferenciamento de bens culturais protegidos</t>
@@ -193,7 +190,7 @@
     <t>Ressarcimentos e contratações temporárias</t>
   </si>
   <si>
-    <t>Contratações temporárias</t>
+    <t>Contratações temporárias e outras despesas de pessoal</t>
   </si>
   <si>
     <t>Implantação do Sistema de Gestão de Processos (BPMS) no Instituto Mineiro de Agropecuária (IMA)</t>
@@ -266,8 +263,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -306,7 +304,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -328,6 +326,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -628,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" zoomScale="55" zoomScaleNormal="55" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -640,9 +644,12 @@
     <col min="2" max="2" width="62.7109375" style="3" customWidth="1"/>
     <col min="3" max="3" width="45" style="3" customWidth="1"/>
     <col min="4" max="4" width="20.85546875" style="6" customWidth="1"/>
-    <col min="5" max="7" width="9.140625" style="3"/>
+    <col min="5" max="5" width="9.140625" style="3"/>
+    <col min="6" max="6" width="16.5703125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="3"/>
     <col min="8" max="8" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="3"/>
+    <col min="9" max="9" width="25.85546875" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -796,7 +803,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="5">
-        <v>3200000</v>
+        <v>4400000</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="20.100000000000001" customHeight="1">
@@ -824,7 +831,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="5">
-        <v>29712000</v>
+        <v>36712000</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="20.100000000000001" customHeight="1">
@@ -1034,7 +1041,7 @@
         <v>5</v>
       </c>
       <c r="D28" s="5">
-        <v>31729352.109999999</v>
+        <v>40729352.109999999</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="20.100000000000001" customHeight="1">
@@ -1093,7 +1100,7 @@
         <v>3072030000</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="33" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A33" s="4">
         <v>9288181</v>
       </c>
@@ -1106,8 +1113,9 @@
       <c r="D33" s="5">
         <v>75352000</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="20.100000000000001" customHeight="1">
+      <c r="I33" s="10"/>
+    </row>
+    <row r="34" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A34" s="4">
         <v>9288182</v>
       </c>
@@ -1121,7 +1129,7 @@
         <v>7000000</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="35" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A35" s="4">
         <v>9288183</v>
       </c>
@@ -1135,7 +1143,7 @@
         <v>9302249.2699999996</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="36" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A36" s="4">
         <v>9288185</v>
       </c>
@@ -1149,7 +1157,7 @@
         <v>2000000</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="37" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A37" s="4">
         <v>9288186</v>
       </c>
@@ -1163,7 +1171,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="38" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A38" s="4">
         <v>9288187</v>
       </c>
@@ -1177,7 +1185,7 @@
         <v>36000000</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="39" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A39" s="4">
         <v>9288188</v>
       </c>
@@ -1191,7 +1199,7 @@
         <v>8647600</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="40" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A40" s="4">
         <v>9288189</v>
       </c>
@@ -1205,7 +1213,7 @@
         <v>300000</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="41" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A41" s="4">
         <v>9288190</v>
       </c>
@@ -1219,7 +1227,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="42" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A42" s="4">
         <v>9288191</v>
       </c>
@@ -1233,7 +1241,7 @@
         <v>210000000</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="43" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A43" s="4">
         <v>9288192</v>
       </c>
@@ -1247,7 +1255,7 @@
         <v>100000000</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="44" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A44" s="4">
         <v>9288193</v>
       </c>
@@ -1261,7 +1269,7 @@
         <v>3900000</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="45" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A45" s="4">
         <v>9288194</v>
       </c>
@@ -1275,7 +1283,7 @@
         <v>3600000</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="46" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A46" s="4">
         <v>9288195</v>
       </c>
@@ -1289,7 +1297,7 @@
         <v>749679</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="47" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A47" s="4">
         <v>9288196</v>
       </c>
@@ -1303,7 +1311,7 @@
         <v>42412000</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="48" spans="1:9" ht="20.100000000000001" customHeight="1">
       <c r="A48" s="4">
         <v>9288198</v>
       </c>
@@ -1317,7 +1325,7 @@
         <v>986059044</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="49" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A49" s="4">
         <v>9288210</v>
       </c>
@@ -1331,7 +1339,7 @@
         <v>2500000</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="50" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A50" s="4">
         <v>9288211</v>
       </c>
@@ -1345,7 +1353,7 @@
         <v>3200000</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="51" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A51" s="4">
         <v>9288212</v>
       </c>
@@ -1356,10 +1364,10 @@
         <v>57</v>
       </c>
       <c r="D51" s="5">
-        <v>2427295557.8899999</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="20.100000000000001" customHeight="1">
+        <v>2427295557.9000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A52" s="4">
         <v>9288213</v>
       </c>
@@ -1373,7 +1381,7 @@
         <v>23000005</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="53" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A53" s="4">
         <v>9321270</v>
       </c>
@@ -1387,7 +1395,7 @@
         <v>842212.06</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="54" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A54">
         <v>9334530</v>
       </c>
@@ -1401,7 +1409,7 @@
         <v>14000000</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="55" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A55">
         <v>9337957</v>
       </c>
@@ -1415,7 +1423,7 @@
         <v>470156273.05000001</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="56" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A56">
         <v>9341846</v>
       </c>
@@ -1429,7 +1437,7 @@
         <v>13900000</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="57" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A57">
         <v>9342884</v>
       </c>
@@ -1443,7 +1451,7 @@
         <v>68000000</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="58" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A58" s="7">
         <v>9361779</v>
       </c>
@@ -1457,7 +1465,7 @@
         <v>164460000</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="20.100000000000001" customHeight="1">
+    <row r="59" spans="1:6" ht="20.100000000000001" customHeight="1">
       <c r="A59" s="7">
         <v>9345390</v>
       </c>
@@ -1470,8 +1478,9 @@
       <c r="D59" s="6">
         <v>24164127.77</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" ht="30">
+      <c r="F59" s="9"/>
+    </row>
+    <row r="60" spans="1:6" ht="30.75">
       <c r="A60" s="7">
         <v>9345097</v>
       </c>
@@ -1485,7 +1494,7 @@
         <v>3091752</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="30">
+    <row r="61" spans="1:6" ht="30.75">
       <c r="A61" s="7">
         <v>9395028</v>
       </c>
@@ -1499,7 +1508,7 @@
         <v>262717753.97999999</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="30.75">
+    <row r="62" spans="1:6" ht="30.75">
       <c r="A62" s="7">
         <v>9428110</v>
       </c>
@@ -1513,7 +1522,7 @@
         <v>200689167</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="30.75">
+    <row r="63" spans="1:6" ht="30.75">
       <c r="A63" s="7">
         <v>9428104</v>
       </c>

</xml_diff>